<commit_message>
Add media, recruitment material. Also revise readme/data dict
</commit_message>
<xml_diff>
--- a/data/dictionary.xlsx
+++ b/data/dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eboumasi\Documents\GitHub\The-Kids-Are-All-Right\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6EC82F5-EB2F-45A6-8311-03B43D3FCFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C5F6AF-2954-4B4B-8EAF-D6C3C67DD194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2736" yWindow="2736" windowWidth="14400" windowHeight="7812" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,9 +54,6 @@
     <t>spotify_tn_selection</t>
   </si>
   <si>
-    <t xml:space="preserve">Comma-separated list of integers. 1 = first legitimate result, 2 = second legitimate result, 3 = third legitimate result, 4 = first clickbait result, 5 = second clickbait result, 6 = third clickbait result, 7 = first scam result, 8 = second scam result , 9 = third scam result, adn 10 = None of the search results </t>
-  </si>
-  <si>
     <t>roblox_tn_selection</t>
   </si>
   <si>
@@ -571,6 +568,9 @@
   </si>
   <si>
     <t>Comma-separated list of categorical variables. Categories correspond to the search result codes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comma-separated list of integers. 1 = first clickbait result, 2 = second clickbait result, 3 = third clickbait result, 4 = first legitimate result, 5 = second legitimate result, 6 = third legitimate result, 7 = first scam result, 8 = second scam result , 9 = third scam result, adn 10 = None of the search results </t>
   </si>
 </sst>
 </file>
@@ -904,19 +904,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.7890625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="31.15625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.734375" style="2"/>
+    <col min="2" max="2" width="24.81640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="31.1796875" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -927,7 +927,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -938,788 +938,789 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" ht="145" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="2" t="s">
+    </row>
+    <row r="7" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="2" t="s">
+    <row r="23" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="B24" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B24" s="2" t="s">
+      <c r="B26" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="2" t="s">
+      <c r="B27" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C27" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="2" t="s">
+      <c r="C28" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C28" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="2" t="s">
+      <c r="C29" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C29" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="2" t="s">
+      <c r="C30" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C30" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="2" t="s">
+      <c r="C31" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C31" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="2" t="s">
+      <c r="C32" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B33" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B33" s="2" t="s">
+      <c r="C35" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B34" s="2" t="s">
+    </row>
+    <row r="37" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B36" s="2" t="s">
+      <c r="C37" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B37" s="2" t="s">
+      <c r="C38" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A40" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B39" s="2" t="s">
+      <c r="C41" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A42" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B40" s="2" t="s">
+      <c r="C42" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A43" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="2" t="s">
+    </row>
+    <row r="44" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A44" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="2" t="s">
+      <c r="C44" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A45" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B45" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A46" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="2" t="s">
+    </row>
+    <row r="47" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A47" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="2" t="s">
+      <c r="C47" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A51" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C50" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="2" t="s">
+      <c r="C51" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A52" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C51" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="2" t="s">
+      <c r="C52" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A53" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C52" s="2" t="s">
+      <c r="B53" s="2" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" s="2" t="s">
+      <c r="C53" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A54" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B53" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C53" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="2" t="s">
+      <c r="C54" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A55" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B54" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="C54" s="2" t="s">
+      <c r="B55" s="2" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="2" t="s">
+      <c r="C55" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A56" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C55" s="2" t="s">
+      <c r="B56" s="2" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" s="2" t="s">
+      <c r="C56" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A57" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B56" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C56" s="2" t="s">
+      <c r="B57" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" s="2" t="s">
+    <row r="58" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A58" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B58" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="115.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" s="2" t="s">
+    </row>
+    <row r="59" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A59" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B59" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" s="2" t="s">
+      <c r="C59" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A60" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B60" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>162</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A62" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B62" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C62" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A63" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" s="2" t="s">
+      <c r="C63" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A64" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B63" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="C63" s="2" t="s">
+      <c r="B64" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A64" s="2" t="s">
+      <c r="C64" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A65" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B64" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C64" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A65" s="2" t="s">
+      <c r="C65" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A66" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B65" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="C65" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A66" s="2" t="s">
+      <c r="C66" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A67" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A67" s="2" t="s">
+      <c r="C67" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A68" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C67" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A68" s="2" t="s">
+      <c r="C68" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A69" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C68" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A69" s="2" t="s">
+      <c r="C69" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A70" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B70" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A71" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B71" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C69" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A70" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B70" s="2" t="s">
+      <c r="C71" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A72" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C70" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A71" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B71" s="2" t="s">
+      <c r="C72" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C71" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A72" s="2" t="s">
+    </row>
+    <row r="73" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A73" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C72" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A73" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B73" s="2" t="s">
+      <c r="C73" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>181</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add other/comment columns to data
</commit_message>
<xml_diff>
--- a/data/dictionary.xlsx
+++ b/data/dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eboumasi\Documents\GitHub\The-Kids-Are-All-Right\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA25F66E-66AB-489C-885A-B611C4D24F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E287F3E4-2A23-413F-80A4-1CC6446A3093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="195">
   <si>
     <t>Column Name</t>
   </si>
@@ -574,6 +574,42 @@
   </si>
   <si>
     <t>Comma-separated list of categorical variables. Categories correspond to the video and website codess defined in the Appendix of the paper</t>
+  </si>
+  <si>
+    <t>scam_other_text</t>
+  </si>
+  <si>
+    <t>scam_comment_text</t>
+  </si>
+  <si>
+    <t>Text response for participants who selected "Leave a comment on the video (please specify)" in Q12 for scam stimuli</t>
+  </si>
+  <si>
+    <t>Text response for participants who selected "Other (please specify)" in Q12 for scam stimuli</t>
+  </si>
+  <si>
+    <t>legit_comment_text</t>
+  </si>
+  <si>
+    <t>legit_other_text</t>
+  </si>
+  <si>
+    <t>Text response for participants who selected "Leave a comment on the video (please specify)" in Q12 for legit stimuli</t>
+  </si>
+  <si>
+    <t>Text response for participants who selected "Other (please specify)" in Q12 for legit stimuli</t>
+  </si>
+  <si>
+    <t>lgt_web_other_text</t>
+  </si>
+  <si>
+    <t>Text response for participants who selected "Other (please specify)" in Q15 for legit stimuli</t>
+  </si>
+  <si>
+    <t>scm_web_other_text</t>
+  </si>
+  <si>
+    <t>Text response for participants who selected "Other (please specify)" in Q15 for scam stimuli</t>
   </si>
 </sst>
 </file>
@@ -905,10 +941,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:C79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1029,78 +1065,78 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="C13" s="2" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>39</v>
+        <v>193</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>33</v>
+        <v>194</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>14</v>
@@ -1108,10 +1144,10 @@
     </row>
     <row r="18" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>14</v>
@@ -1119,32 +1155,32 @@
     </row>
     <row r="19" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>43</v>
+        <v>187</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>37</v>
+        <v>189</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>44</v>
+        <v>188</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>38</v>
+        <v>190</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>14</v>
@@ -1152,54 +1188,54 @@
     </row>
     <row r="22" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>57</v>
+        <v>191</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>58</v>
+        <v>192</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>14</v>
@@ -1207,518 +1243,584 @@
     </row>
     <row r="27" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>110</v>
+        <v>38</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>111</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
+    <row r="35" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
+    <row r="36" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A31" s="2" t="s">
+    <row r="37" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="58" x14ac:dyDescent="0.35">
-      <c r="A39" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C41" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="58" x14ac:dyDescent="0.35">
-      <c r="A42" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>7</v>
+        <v>133</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>153</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A57" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A58" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A59" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A60" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A61" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A62" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B62" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C62" s="2" t="s">
         <v>155</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="58" x14ac:dyDescent="0.35">
-      <c r="A57" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A58" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="58" x14ac:dyDescent="0.35">
-      <c r="A60" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="58" x14ac:dyDescent="0.35">
-      <c r="A61" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A62" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>170</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A67" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A68" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A69" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A70" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A71" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A72" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A67" s="2" t="s">
+      <c r="C72" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A73" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C73" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A68" s="2" t="s">
+    <row r="74" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A74" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C74" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A69" s="2" t="s">
+    <row r="75" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A75" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B75" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C75" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A70" s="2" t="s">
+    <row r="76" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A76" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B76" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C76" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A71" s="2" t="s">
+    <row r="77" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A77" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C77" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A72" s="2" t="s">
+    <row r="78" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A78" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C78" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="58" x14ac:dyDescent="0.35">
-      <c r="A73" s="2" t="s">
+    <row r="79" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A79" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B79" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C79" s="2" t="s">
         <v>180</v>
       </c>
     </row>

</xml_diff>